<commit_message>
All files added and output saved at selected location
</commit_message>
<xml_diff>
--- a/CSAY_DipGen/CSAY_DipGen/Direct purchase docs record.xlsx
+++ b/CSAY_DipGen/CSAY_DipGen/Direct purchase docs record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_DipGEN\CSAY_DipGen\CSAY_DipGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7200E62-5632-4756-A66B-E5769ADF5E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C45DAE-1F90-4714-BE27-E0D765F549FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct purchase" sheetId="1" r:id="rId1"/>
@@ -1179,45 +1179,6 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1226,6 +1187,45 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1650,14 +1650,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2380,7 +2380,7 @@
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A18" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C24"/>
     </sheetView>
   </sheetViews>
@@ -2397,14 +2397,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -3316,81 +3316,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
     </row>
     <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -3404,16 +3404,16 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="58" t="s">
         <v>111</v>
       </c>
       <c r="E6" s="41" t="s">
@@ -3437,10 +3437,10 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="21" t="s">
         <v>114</v>
       </c>
@@ -3696,13 +3696,13 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
       <c r="F14" s="36">
         <f>ROUND(SUM(F9:F13),2)</f>
         <v>794635.48</v>
@@ -3725,13 +3725,13 @@
       <c r="M14" s="30"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="36">
         <f>ROUND(F14*0.13,2)</f>
         <v>103302.61</v>
@@ -3754,13 +3754,13 @@
       <c r="M15" s="30"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="54"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="36">
         <f>ROUND(F14+F15,2)</f>
         <v>897938.09</v>
@@ -3783,13 +3783,13 @@
       <c r="M16" s="30"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29">
@@ -3809,13 +3809,13 @@
       <c r="M17" s="30"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="31">
@@ -3835,13 +3835,13 @@
       <c r="M18" s="30"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="32">
@@ -3877,12 +3877,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -3892,6 +3886,12 @@
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3901,7 +3901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72F8C71-938A-46C4-A864-C1DC75B54701}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3911,42 +3911,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="47" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="42" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.6">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="48" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="43" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="44" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="23.25" x14ac:dyDescent="0.6">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="49" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="45" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="24" x14ac:dyDescent="0.6">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="46" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>